<commit_message>
logos eur gbp usd changed
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27049,21</t>
+          <t>27158,77</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>4,2686</t>
+          <t>4,2568</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>1556,76</t>
+          <t>1569,28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
some gui performance upgrade, fetch error info patched
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27158,77</t>
+          <t>26797,47</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>4,2568</t>
+          <t>4,2552</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>1569,28</t>
+          <t>1560,03</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
etf fetching changed to marketwatch
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -685,7 +685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>ethereum</t>
+          <t>emim-etf</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>swda-etf</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
@@ -776,7 +776,11 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
       <c r="G2" s="3" t="inlineStr"/>
@@ -795,7 +799,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>A23</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -803,7 +807,11 @@
           <t>A4</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr"/>
@@ -822,7 +830,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
top bar buttons design changed
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>26797,47</t>
+          <t>26796,89</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>4,2552</t>
+          <t>4,3165</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>emim-etf</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>swda-etf</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
@@ -763,24 +763,20 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
+          <t>Arkusz3</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
       <c r="G2" s="3" t="inlineStr"/>
@@ -799,19 +795,15 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
+          <t>A5</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
           <t>A4</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A4</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
+      <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr"/>
@@ -830,7 +822,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -840,7 +832,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -928,7 +920,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>1588,65</t>
+          <t>26838,56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
etfs fetch page changed again..
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -499,7 +499,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>0,5243</t>
+          <t>6773,0</t>
         </is>
       </c>
     </row>
@@ -513,14 +513,14 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>4,3177</t>
+          <t>4,3065</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.8" customHeight="1" s="2">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>1891,6</t>
+          <t>1910,8</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A5</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr"/>
@@ -928,7 +928,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>26780,6</t>
+          <t>26851,54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
gui update, hint text added to buttons on topbar
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -513,7 +513,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>4,2607</t>
+          <t>4,2457</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>emim-etf</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -728,12 +728,12 @@
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>silver</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>ethereum</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
@@ -783,26 +783,14 @@
           <t>Arkusz3</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="D2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
       <c r="G2" s="3" t="inlineStr"/>
       <c r="H2" s="3" t="inlineStr"/>
@@ -818,26 +806,14 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
+      <c r="B3" s="3" t="inlineStr"/>
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>A4</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>B7</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>V55</t>
-        </is>
-      </c>
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr"/>
       <c r="H3" s="3" t="inlineStr"/>
@@ -953,7 +929,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27762,88</t>
+          <t>27729,26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
metal scrapping page update
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -499,7 +499,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2926,085</t>
+          <t>2455,0</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>4,2457</t>
+          <t>3,976</t>
         </is>
       </c>
     </row>
@@ -702,7 +702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
@@ -713,17 +713,17 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>bitcoin</t>
+          <t>xag</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
+          <t>xau</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
           <t>-</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>usd</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -780,15 +780,15 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Arkusz3</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr"/>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
           <t>Sheet1</t>
         </is>
       </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
@@ -806,12 +806,12 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A4</t>
-        </is>
-      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
@@ -841,7 +841,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -929,7 +929,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27729,26</t>
+          <t>41893,09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
api button added and logic
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>26796,89</t>
+          <t>43614,21</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -702,7 +702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
@@ -713,12 +713,12 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>xag</t>
+          <t>bitcoin</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>xau</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -783,11 +783,7 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
@@ -806,11 +802,7 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>V4</t>
-        </is>
-      </c>
+      <c r="B3" s="3" t="inlineStr"/>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>

</xml_diff>

<commit_message>
update api and non api fix
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -702,7 +702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
@@ -718,7 +718,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>holyheld-2</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -783,7 +783,11 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
@@ -802,7 +806,11 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>

</xml_diff>